<commit_message>
data source update & load complete
</commit_message>
<xml_diff>
--- a/Data Sources.xlsx
+++ b/Data Sources.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Learning Files\OneDrive - University of Leeds\College\Study in UoL\Semester 2\GEOG5990M Programming for Geographical Information Analysis-Core Skills\Assignment final project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D12DDAD8-3624-410B-9DC0-DFF5FFDE1A33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61B64873-4471-445F-8777-8281D76DAFBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
   <si>
     <t>No.</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -106,6 +106,10 @@
   </si>
   <si>
     <t>this zip file's original name from download site is too long, might cause windows file exploer broken. Rename it before directly open it or during running code</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">contains the </t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -445,7 +449,7 @@
   <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -489,8 +493,11 @@
       <c r="C2" t="s">
         <v>18</v>
       </c>
+      <c r="D2" t="s">
+        <v>21</v>
+      </c>
       <c r="E2" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>5</v>

</xml_diff>